<commit_message>
Added items for Oneplus 6t
</commit_message>
<xml_diff>
--- a/Wishlist.xlsx
+++ b/Wishlist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CF2CF8-502D-4E74-8D06-9C7951A11F65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282266F3-DFF0-4C2D-984E-0F6506DBBDC1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Item_Nr.</t>
   </si>
@@ -59,6 +59,21 @@
   </si>
   <si>
     <t>Stirnlampe</t>
+  </si>
+  <si>
+    <t>https://www.bauhaus.info/stirnlampen/profi-depot-stirnlampe/p/25568884</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/s?k=oneplus+6t+panzerglas&amp;__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=2O2D66FWAGP4K&amp;sprefix=oneplus+6t+%2Caps%2C190&amp;ref=nb_sb_ss_i_3_11</t>
+  </si>
+  <si>
+    <t>Rhinoshield solidsuit schutzhülle oneplus 6t</t>
+  </si>
+  <si>
+    <t>Schutzfolie/Panzerglas Oneplus 6t</t>
+  </si>
+  <si>
+    <t>https://rhinoshield.de/pages/shop/OnePlus?device=oneplus-6t&amp;category=solidsuit&amp;collection=solidsuit-android</t>
   </si>
 </sst>
 </file>
@@ -457,12 +472,12 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="90.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -546,23 +561,37 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">

</xml_diff>